<commit_message>
book list 2024 update
</commit_message>
<xml_diff>
--- a/content/My Book Library.xlsx
+++ b/content/My Book Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\qprop_blog\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417092C1-6B03-418F-BDF2-A1FAA323EC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2682A3FB-179C-40B0-92C3-5F4548676DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="193">
   <si>
     <t>Book Name</t>
   </si>
@@ -561,6 +561,48 @@
   </si>
   <si>
     <t>Eric Schmidt &amp; Jonathan Rosenberg</t>
+  </si>
+  <si>
+    <t>Essentialism</t>
+  </si>
+  <si>
+    <t>Greg McKeown</t>
+  </si>
+  <si>
+    <t>Selfhelp</t>
+  </si>
+  <si>
+    <t>The Good Success</t>
+  </si>
+  <si>
+    <t>Dr Emmanuel Mango</t>
+  </si>
+  <si>
+    <t>Failing Forward</t>
+  </si>
+  <si>
+    <t>The Prize: The Epic Quest for Oil, Money &amp; Power</t>
+  </si>
+  <si>
+    <t>Daniel Yergin</t>
+  </si>
+  <si>
+    <t>Why (Not) Me: Memoir</t>
+  </si>
+  <si>
+    <t>John C Gichinga</t>
+  </si>
+  <si>
+    <t>One Night at the Call Centre</t>
+  </si>
+  <si>
+    <t>Chetan Bhagat</t>
+  </si>
+  <si>
+    <t>The flame trees of Thika</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elspeth Huxley</t>
   </si>
 </sst>
 </file>
@@ -630,9 +672,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -670,7 +712,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -776,7 +818,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -918,7 +960,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -926,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,6 +2027,104 @@
       </c>
       <c r="D75" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>179</v>
+      </c>
+      <c r="B76" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" s="3">
+        <v>45540</v>
+      </c>
+      <c r="D76" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>182</v>
+      </c>
+      <c r="B77" t="s">
+        <v>183</v>
+      </c>
+      <c r="C77" s="3">
+        <v>45447</v>
+      </c>
+      <c r="D77" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>184</v>
+      </c>
+      <c r="B78" t="s">
+        <v>106</v>
+      </c>
+      <c r="C78" s="3">
+        <v>45494</v>
+      </c>
+      <c r="D78" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>185</v>
+      </c>
+      <c r="B79" t="s">
+        <v>186</v>
+      </c>
+      <c r="C79" s="3">
+        <v>45272</v>
+      </c>
+      <c r="D79" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>187</v>
+      </c>
+      <c r="B80" t="s">
+        <v>188</v>
+      </c>
+      <c r="C80" s="3">
+        <v>45303</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>189</v>
+      </c>
+      <c r="B81" t="s">
+        <v>190</v>
+      </c>
+      <c r="C81" s="3">
+        <v>44573</v>
+      </c>
+      <c r="D81" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>191</v>
+      </c>
+      <c r="B82" t="s">
+        <v>192</v>
+      </c>
+      <c r="C82" s="3">
+        <v>44573</v>
+      </c>
+      <c r="D82" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>